<commit_message>
se añadieron varias librerias de xlsx para poder controlar y hacer pruebas con archivos, se implemetno modulos de next.config para quitar errores del mismo next, se añadio una api que nos retorna un link para obtener un plantilla de los formatos empleados en la empresa
</commit_message>
<xml_diff>
--- a/plantilla.xlsx
+++ b/plantilla.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBBCC3A-846B-4EC5-A7BB-0E86CA838C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81C0BF4-37D0-4675-BD01-D430C11DC7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{49BB519B-A59E-4961-917A-B4F658F6CFD5}"/>
+    <workbookView xWindow="4725" yWindow="4395" windowWidth="28800" windowHeight="15285" xr2:uid="{49BB519B-A59E-4961-917A-B4F658F6CFD5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
-    <sheet name="requisicion" sheetId="3" r:id="rId2"/>
+    <sheet name="hola" sheetId="4" r:id="rId1"/>
+    <sheet name="asdf" sheetId="3" r:id="rId2"/>
     <sheet name="ordenCompra" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">asdf!$A$1:$Q$40</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">ordenCompra!$B$1:$M$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">requisicion!$A$1:$Q$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="93">
   <si>
     <t xml:space="preserve">O R D E N   D E   C O M P R A. </t>
   </si>
@@ -1730,6 +1730,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1757,9 +1760,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1769,6 +1769,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1778,24 +1796,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1835,116 +1835,56 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2030,38 +1970,98 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="76" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="55" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="57" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="58" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2085,6 +2085,154 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>100852</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2151528" cy="515472"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAECB6C6-C828-4DCE-BF77-A32162096047}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="100852" y="251572"/>
+          <a:ext cx="2151528" cy="515472"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302558</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>202265</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>18490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Un dibujo de una persona&#10;&#10;Descripción generada automáticamente con confianza media">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75597BB5-812F-496C-9A64-7925A333623D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="474008" y="7733740"/>
+          <a:ext cx="1118907" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2232,7 +2380,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2684,15 +2832,998 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6928D101-F899-4DCB-B278-529DF970D7DA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.25">
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="183" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
+      <c r="N2" s="183"/>
+      <c r="O2" s="183"/>
+      <c r="P2" s="95"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="184" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="184"/>
+      <c r="O3" s="184"/>
+      <c r="P3" s="95"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75">
+      <c r="A5" s="94"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="185"/>
+      <c r="K5" s="185"/>
+      <c r="L5" s="186" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="186"/>
+      <c r="N5" s="186"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="97"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75">
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="185"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="94"/>
+      <c r="B7" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="181"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="188" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="188"/>
+      <c r="P7" s="188"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="94"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="104"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="94"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="94"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="94"/>
+      <c r="B9" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="104"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="104" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="94"/>
+      <c r="P9" s="103"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="94"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="104"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="94"/>
+      <c r="P10" s="103"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="94"/>
+      <c r="B11" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="182"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
+      <c r="G11" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="103"/>
+      <c r="I11" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="104"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="104" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" s="94"/>
+      <c r="P11" s="103"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="104" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="104"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="94"/>
+      <c r="O12" s="94"/>
+      <c r="P12" s="94"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="104"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="104"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="94"/>
+      <c r="O15" s="94"/>
+      <c r="P15" s="94"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="94"/>
+      <c r="B17" s="170" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="172" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="172" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="170" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="170" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="170" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" s="172" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="173"/>
+      <c r="O17" s="173"/>
+      <c r="P17" s="174"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="94"/>
+      <c r="B18" s="171"/>
+      <c r="C18" s="107" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="175"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="175"/>
+      <c r="J18" s="171"/>
+      <c r="K18" s="171"/>
+      <c r="L18" s="171"/>
+      <c r="M18" s="175"/>
+      <c r="N18" s="176"/>
+      <c r="O18" s="176"/>
+      <c r="P18" s="177"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="94"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="94"/>
+      <c r="B20" s="109">
+        <v>1</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="178"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="167"/>
+      <c r="N20" s="168"/>
+      <c r="O20" s="168"/>
+      <c r="P20" s="169"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="94"/>
+      <c r="B21" s="114">
+        <v>2</v>
+      </c>
+      <c r="C21" s="114"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="163"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="117"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="164"/>
+      <c r="N21" s="165"/>
+      <c r="O21" s="165"/>
+      <c r="P21" s="166"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="94"/>
+      <c r="B22" s="114">
+        <v>3</v>
+      </c>
+      <c r="C22" s="114"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
+      <c r="H22" s="169"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="158"/>
+      <c r="N22" s="159"/>
+      <c r="O22" s="159"/>
+      <c r="P22" s="160"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="94"/>
+      <c r="B23" s="114">
+        <f t="shared" ref="B23:B30" si="0">+B22+1</f>
+        <v>4</v>
+      </c>
+      <c r="C23" s="114"/>
+      <c r="D23" s="158"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="115"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="158"/>
+      <c r="N23" s="159"/>
+      <c r="O23" s="159"/>
+      <c r="P23" s="160"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="94"/>
+      <c r="B24" s="114">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="114"/>
+      <c r="D24" s="158"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="118">
+        <f>SUM(K20:K22)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="119"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="153"/>
+      <c r="O24" s="153"/>
+      <c r="P24" s="154"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="94"/>
+      <c r="B25" s="114">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C25" s="114"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="159"/>
+      <c r="F25" s="159"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="114"/>
+      <c r="J25" s="114"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="119"/>
+      <c r="M25" s="152"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="154"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="94"/>
+      <c r="B26" s="114">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C26" s="114"/>
+      <c r="D26" s="158"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="114"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="158"/>
+      <c r="N26" s="159"/>
+      <c r="O26" s="159"/>
+      <c r="P26" s="160"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="94"/>
+      <c r="B27" s="114">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C27" s="122"/>
+      <c r="D27" s="149" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="150"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" s="120">
+        <f>K24*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" s="152"/>
+      <c r="N27" s="153"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="154"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="94"/>
+      <c r="B28" s="114">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C28" s="122"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="152"/>
+      <c r="N28" s="153"/>
+      <c r="O28" s="153"/>
+      <c r="P28" s="154"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="94"/>
+      <c r="B29" s="114">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C29" s="122"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="122"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="122"/>
+      <c r="L29" s="122"/>
+      <c r="M29" s="124"/>
+      <c r="N29" s="125"/>
+      <c r="O29" s="125"/>
+      <c r="P29" s="126"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="94"/>
+      <c r="B30" s="127">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C30" s="128"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="157"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="128"/>
+      <c r="L30" s="128"/>
+      <c r="M30" s="129" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="130"/>
+      <c r="O30" s="130"/>
+      <c r="P30" s="131"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="94"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="133">
+        <f>K24+K27</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
+      <c r="N31" s="134"/>
+      <c r="O31" s="132"/>
+      <c r="P31" s="132"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="94"/>
+      <c r="B32" s="147" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="147"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="135" t="s">
+        <v>74</v>
+      </c>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="94"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="135"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="135"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="94"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="94"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="135"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="94"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="94"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="135"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="135"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="94"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="94"/>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="94"/>
+      <c r="N36" s="135"/>
+      <c r="O36" s="94"/>
+      <c r="P36" s="94"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="135"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="135"/>
+      <c r="O37" s="94"/>
+      <c r="P37" s="94"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="94"/>
+      <c r="B38" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="148"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="136" t="s">
+        <v>77</v>
+      </c>
+      <c r="K38" s="135"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="135" t="s">
+        <v>78</v>
+      </c>
+      <c r="O38" s="94"/>
+      <c r="P38" s="94"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="94"/>
+      <c r="B39" s="147" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="147"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="137" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="138"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="139" t="s">
+        <v>81</v>
+      </c>
+      <c r="K39" s="135"/>
+      <c r="L39" s="94"/>
+      <c r="M39" s="136"/>
+      <c r="N39" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="O39" s="136"/>
+      <c r="P39" s="94"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="94"/>
+      <c r="B40" s="94"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="94"/>
+      <c r="I40" s="94"/>
+      <c r="J40" s="94"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="94"/>
+      <c r="M40" s="94"/>
+      <c r="N40" s="135"/>
+      <c r="O40" s="94"/>
+      <c r="P40" s="94"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="94"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="94"/>
+      <c r="I41" s="94"/>
+      <c r="J41" s="94"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="94"/>
+      <c r="M41" s="94"/>
+      <c r="N41" s="94"/>
+      <c r="O41" s="94"/>
+      <c r="P41" s="94"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="94"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="94"/>
+      <c r="I42" s="94"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="94"/>
+      <c r="L42" s="94"/>
+      <c r="M42" s="94"/>
+      <c r="N42" s="94"/>
+      <c r="O42" s="94"/>
+      <c r="P42" s="94"/>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="94"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="94"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="94"/>
+      <c r="I43" s="94"/>
+      <c r="J43" s="94"/>
+      <c r="K43" s="94"/>
+      <c r="L43" s="94"/>
+      <c r="M43" s="94"/>
+      <c r="N43" s="94"/>
+      <c r="O43" s="94"/>
+      <c r="P43" s="94"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="94"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="94"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94"/>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="94"/>
+      <c r="N44" s="94"/>
+      <c r="O44" s="94"/>
+      <c r="P44" s="94"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="94"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="94"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="94"/>
+      <c r="M45" s="94"/>
+      <c r="N45" s="94"/>
+      <c r="O45" s="94"/>
+      <c r="P45" s="94"/>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="F2:O2"/>
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:P18"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2704,7 +3835,7 @@
   <dimension ref="B2:V40"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="P45" sqref="A1:P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3674,64 +4805,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="20.25" customHeight="1">
-      <c r="F2" s="184" t="s">
+      <c r="F2" s="183" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184"/>
-      <c r="O2" s="184"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
+      <c r="N2" s="183"/>
+      <c r="O2" s="183"/>
       <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:16" ht="35.25" customHeight="1">
-      <c r="F3" s="185" t="s">
+      <c r="F3" s="184" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="185"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="184"/>
+      <c r="O3" s="184"/>
       <c r="P3" s="95"/>
     </row>
     <row r="4" spans="2:16" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:16" ht="15.75">
       <c r="B5" s="96"/>
       <c r="C5" s="96"/>
-      <c r="D5" s="186"/>
-      <c r="E5" s="186"/>
-      <c r="F5" s="186"/>
-      <c r="G5" s="186"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="186"/>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186"/>
-      <c r="L5" s="187" t="s">
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="185"/>
+      <c r="K5" s="185"/>
+      <c r="L5" s="186" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="188"/>
+      <c r="M5" s="186"/>
+      <c r="N5" s="186"/>
+      <c r="O5" s="187"/>
       <c r="P5" s="97"/>
     </row>
     <row r="6" spans="2:16" ht="15.75">
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="186"/>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="186"/>
-      <c r="K6" s="186"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="185"/>
       <c r="L6" s="98"/>
     </row>
     <row r="7" spans="2:16">
@@ -3750,11 +4881,11 @@
       <c r="K7" s="101"/>
       <c r="L7" s="101"/>
       <c r="M7" s="102"/>
-      <c r="N7" s="183" t="s">
+      <c r="N7" s="188" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="183"/>
-      <c r="P7" s="183"/>
+      <c r="O7" s="188"/>
+      <c r="P7" s="188"/>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1">
       <c r="B8" s="99"/>
@@ -3923,40 +5054,40 @@
       <c r="J20" s="111"/>
       <c r="K20" s="112"/>
       <c r="L20" s="113"/>
-      <c r="M20" s="161"/>
-      <c r="N20" s="162"/>
-      <c r="O20" s="162"/>
-      <c r="P20" s="163"/>
+      <c r="M20" s="167"/>
+      <c r="N20" s="168"/>
+      <c r="O20" s="168"/>
+      <c r="P20" s="169"/>
     </row>
     <row r="21" spans="2:22" ht="43.5" customHeight="1">
       <c r="B21" s="114">
         <v>2</v>
       </c>
       <c r="C21" s="114"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="165"/>
-      <c r="F21" s="165"/>
-      <c r="G21" s="165"/>
-      <c r="H21" s="166"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="163"/>
       <c r="I21" s="115"/>
       <c r="J21" s="116"/>
       <c r="K21" s="117"/>
       <c r="L21" s="114"/>
-      <c r="M21" s="167"/>
-      <c r="N21" s="168"/>
-      <c r="O21" s="168"/>
-      <c r="P21" s="169"/>
+      <c r="M21" s="164"/>
+      <c r="N21" s="165"/>
+      <c r="O21" s="165"/>
+      <c r="P21" s="166"/>
     </row>
     <row r="22" spans="2:22" ht="26.25" customHeight="1">
       <c r="B22" s="114">
         <v>3</v>
       </c>
       <c r="C22" s="114"/>
-      <c r="D22" s="161"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="162"/>
-      <c r="H22" s="163"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="115"/>
       <c r="J22" s="116"/>
       <c r="K22" s="117"/>
@@ -4006,10 +5137,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="119"/>
-      <c r="M24" s="151"/>
-      <c r="N24" s="152"/>
-      <c r="O24" s="152"/>
-      <c r="P24" s="153"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="153"/>
+      <c r="O24" s="153"/>
+      <c r="P24" s="154"/>
     </row>
     <row r="25" spans="2:22" ht="21" customHeight="1">
       <c r="B25" s="114">
@@ -4026,10 +5157,10 @@
       <c r="J25" s="114"/>
       <c r="K25" s="120"/>
       <c r="L25" s="119"/>
-      <c r="M25" s="151"/>
-      <c r="N25" s="152"/>
-      <c r="O25" s="152"/>
-      <c r="P25" s="153"/>
+      <c r="M25" s="152"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="154"/>
     </row>
     <row r="26" spans="2:22" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="114">
@@ -4057,13 +5188,13 @@
         <v>8</v>
       </c>
       <c r="C27" s="122"/>
-      <c r="D27" s="148" t="s">
+      <c r="D27" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="149"/>
-      <c r="H27" s="150"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="151"/>
       <c r="I27" s="122"/>
       <c r="J27" s="114" t="s">
         <v>41</v>
@@ -4075,10 +5206,10 @@
       <c r="L27" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="M27" s="151"/>
-      <c r="N27" s="152"/>
-      <c r="O27" s="152"/>
-      <c r="P27" s="153"/>
+      <c r="M27" s="152"/>
+      <c r="N27" s="153"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="154"/>
     </row>
     <row r="28" spans="2:22" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="114">
@@ -4086,19 +5217,19 @@
         <v>9</v>
       </c>
       <c r="C28" s="122"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="149"/>
-      <c r="H28" s="150"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="151"/>
       <c r="I28" s="122"/>
       <c r="J28" s="122"/>
       <c r="K28" s="123"/>
       <c r="L28" s="122"/>
-      <c r="M28" s="151"/>
-      <c r="N28" s="152"/>
-      <c r="O28" s="152"/>
-      <c r="P28" s="153"/>
+      <c r="M28" s="152"/>
+      <c r="N28" s="153"/>
+      <c r="O28" s="153"/>
+      <c r="P28" s="154"/>
     </row>
     <row r="29" spans="2:22" ht="20.100000000000001" customHeight="1">
       <c r="B29" s="114">
@@ -4106,11 +5237,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="122"/>
-      <c r="D29" s="148"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="149"/>
-      <c r="H29" s="150"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="151"/>
       <c r="I29" s="122"/>
       <c r="J29" s="122"/>
       <c r="K29" s="122"/>
@@ -4126,11 +5257,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="128"/>
-      <c r="D30" s="154"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
-      <c r="H30" s="156"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="157"/>
       <c r="I30" s="128"/>
       <c r="J30" s="128"/>
       <c r="K30" s="128"/>
@@ -4207,12 +5338,12 @@
       <c r="B38" s="94" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="157" t="s">
+      <c r="E38" s="148" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="157"/>
-      <c r="G38" s="157"/>
-      <c r="H38" s="157"/>
+      <c r="F38" s="148"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="148"/>
       <c r="J38" s="136" t="s">
         <v>77</v>
       </c>
@@ -4246,13 +5377,25 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="F2:O2"/>
-    <mergeCell ref="F3:O3"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M24:P24"/>
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="M21:P21"/>
     <mergeCell ref="D8:F8"/>
@@ -4267,25 +5410,13 @@
     <mergeCell ref="M20:P20"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="F2:O2"/>
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -5145,15 +6276,15 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="252" t="s">
+      <c r="E1" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="252"/>
-      <c r="I1" s="252"/>
-      <c r="J1" s="252"/>
-      <c r="K1" s="252"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3" t="s">
         <v>1</v>
@@ -5178,19 +6309,19 @@
       <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="253" t="s">
+      <c r="C4" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="253"/>
-      <c r="E4" s="253"/>
-      <c r="F4" s="254"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
+      <c r="F4" s="193"/>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="255"/>
-      <c r="I4" s="255"/>
-      <c r="J4" s="255"/>
-      <c r="K4" s="256"/>
+      <c r="H4" s="194"/>
+      <c r="I4" s="194"/>
+      <c r="J4" s="194"/>
+      <c r="K4" s="195"/>
       <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
@@ -5200,37 +6331,37 @@
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="257" t="s">
+      <c r="C5" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="257"/>
-      <c r="E5" s="257"/>
-      <c r="F5" s="258"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="196"/>
+      <c r="F5" s="197"/>
       <c r="G5" s="140" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="259"/>
-      <c r="I5" s="259"/>
-      <c r="J5" s="259"/>
-      <c r="K5" s="260"/>
-      <c r="L5" s="250"/>
-      <c r="M5" s="251"/>
+      <c r="H5" s="198"/>
+      <c r="I5" s="198"/>
+      <c r="J5" s="198"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="189"/>
+      <c r="M5" s="190"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="226" t="s">
+      <c r="B6" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="227"/>
-      <c r="D6" s="227"/>
-      <c r="E6" s="227"/>
-      <c r="F6" s="228"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="208"/>
       <c r="G6" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="244"/>
-      <c r="I6" s="244"/>
-      <c r="J6" s="244"/>
-      <c r="K6" s="245"/>
+      <c r="H6" s="224"/>
+      <c r="I6" s="224"/>
+      <c r="J6" s="224"/>
+      <c r="K6" s="225"/>
       <c r="L6" s="17" t="s">
         <v>11</v>
       </c>
@@ -5249,52 +6380,52 @@
       <c r="G7" s="143" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="247"/>
-      <c r="L7" s="229"/>
-      <c r="M7" s="230"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="227"/>
+      <c r="L7" s="209"/>
+      <c r="M7" s="210"/>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="227"/>
-      <c r="D8" s="227"/>
-      <c r="E8" s="227"/>
-      <c r="F8" s="227"/>
-      <c r="G8" s="231" t="s">
+      <c r="C8" s="207"/>
+      <c r="D8" s="207"/>
+      <c r="E8" s="207"/>
+      <c r="F8" s="207"/>
+      <c r="G8" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="232"/>
-      <c r="I8" s="233" t="s">
+      <c r="H8" s="212"/>
+      <c r="I8" s="213" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="234"/>
-      <c r="K8" s="235"/>
+      <c r="J8" s="214"/>
+      <c r="K8" s="215"/>
       <c r="L8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="M8" s="21"/>
     </row>
     <row r="9" spans="2:13" ht="15" customHeight="1">
-      <c r="B9" s="236"/>
-      <c r="C9" s="237"/>
-      <c r="D9" s="237"/>
-      <c r="E9" s="237"/>
-      <c r="F9" s="238"/>
-      <c r="G9" s="239" t="s">
+      <c r="B9" s="216"/>
+      <c r="C9" s="217"/>
+      <c r="D9" s="217"/>
+      <c r="E9" s="217"/>
+      <c r="F9" s="218"/>
+      <c r="G9" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="240"/>
-      <c r="I9" s="240" t="s">
+      <c r="H9" s="220"/>
+      <c r="I9" s="220" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="240"/>
-      <c r="K9" s="241"/>
-      <c r="L9" s="242"/>
-      <c r="M9" s="243"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="221"/>
+      <c r="L9" s="222"/>
+      <c r="M9" s="223"/>
     </row>
     <row r="10" spans="2:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="B10" s="22"/>
@@ -5305,10 +6436,10 @@
       <c r="G10" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="248"/>
-      <c r="I10" s="248"/>
-      <c r="J10" s="248"/>
-      <c r="K10" s="249"/>
+      <c r="H10" s="228"/>
+      <c r="I10" s="228"/>
+      <c r="J10" s="228"/>
+      <c r="K10" s="229"/>
       <c r="L10" s="25"/>
       <c r="M10" s="26"/>
     </row>
@@ -5339,14 +6470,14 @@
       <c r="E12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="220" t="s">
+      <c r="F12" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="221"/>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="221"/>
-      <c r="K12" s="222"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="201"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="201"/>
+      <c r="K12" s="202"/>
       <c r="L12" s="29" t="s">
         <v>24</v>
       </c>
@@ -5361,12 +6492,12 @@
       <c r="E13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="223"/>
-      <c r="G13" s="224"/>
-      <c r="H13" s="224"/>
-      <c r="I13" s="224"/>
-      <c r="J13" s="224"/>
-      <c r="K13" s="225"/>
+      <c r="F13" s="203"/>
+      <c r="G13" s="204"/>
+      <c r="H13" s="204"/>
+      <c r="I13" s="204"/>
+      <c r="J13" s="204"/>
+      <c r="K13" s="205"/>
       <c r="L13" s="33" t="s">
         <v>27</v>
       </c>
@@ -5377,12 +6508,12 @@
       <c r="C14" s="36"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
-      <c r="F14" s="208"/>
-      <c r="G14" s="209"/>
-      <c r="H14" s="209"/>
-      <c r="I14" s="209"/>
-      <c r="J14" s="209"/>
-      <c r="K14" s="210"/>
+      <c r="F14" s="233"/>
+      <c r="G14" s="234"/>
+      <c r="H14" s="234"/>
+      <c r="I14" s="234"/>
+      <c r="J14" s="234"/>
+      <c r="K14" s="235"/>
       <c r="L14" s="37"/>
       <c r="M14" s="38">
         <f>+C14*L14</f>
@@ -5394,12 +6525,12 @@
       <c r="C15" s="36"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
-      <c r="F15" s="208"/>
-      <c r="G15" s="209"/>
-      <c r="H15" s="209"/>
-      <c r="I15" s="209"/>
-      <c r="J15" s="209"/>
-      <c r="K15" s="210"/>
+      <c r="F15" s="233"/>
+      <c r="G15" s="234"/>
+      <c r="H15" s="234"/>
+      <c r="I15" s="234"/>
+      <c r="J15" s="234"/>
+      <c r="K15" s="235"/>
       <c r="L15" s="37"/>
       <c r="M15" s="38"/>
     </row>
@@ -5408,12 +6539,12 @@
       <c r="C16" s="40"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
-      <c r="F16" s="211"/>
-      <c r="G16" s="212"/>
-      <c r="H16" s="212"/>
-      <c r="I16" s="212"/>
-      <c r="J16" s="212"/>
-      <c r="K16" s="213"/>
+      <c r="F16" s="236"/>
+      <c r="G16" s="237"/>
+      <c r="H16" s="237"/>
+      <c r="I16" s="237"/>
+      <c r="J16" s="237"/>
+      <c r="K16" s="238"/>
       <c r="L16" s="37"/>
       <c r="M16" s="38"/>
     </row>
@@ -5422,12 +6553,12 @@
       <c r="C17" s="40"/>
       <c r="D17" s="33"/>
       <c r="E17" s="41"/>
-      <c r="F17" s="208"/>
-      <c r="G17" s="209"/>
-      <c r="H17" s="209"/>
-      <c r="I17" s="209"/>
-      <c r="J17" s="209"/>
-      <c r="K17" s="210"/>
+      <c r="F17" s="233"/>
+      <c r="G17" s="234"/>
+      <c r="H17" s="234"/>
+      <c r="I17" s="234"/>
+      <c r="J17" s="234"/>
+      <c r="K17" s="235"/>
       <c r="L17" s="37"/>
       <c r="M17" s="38"/>
     </row>
@@ -5436,12 +6567,12 @@
       <c r="C18" s="40"/>
       <c r="D18" s="33"/>
       <c r="E18" s="41"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="215"/>
-      <c r="H18" s="215"/>
-      <c r="I18" s="215"/>
-      <c r="J18" s="215"/>
-      <c r="K18" s="216"/>
+      <c r="F18" s="239"/>
+      <c r="G18" s="240"/>
+      <c r="H18" s="240"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="241"/>
       <c r="L18" s="37"/>
       <c r="M18" s="38"/>
     </row>
@@ -5450,14 +6581,14 @@
       <c r="C19" s="40"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
-      <c r="F19" s="214" t="s">
+      <c r="F19" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="215"/>
-      <c r="H19" s="215"/>
-      <c r="I19" s="215"/>
-      <c r="J19" s="215"/>
-      <c r="K19" s="216"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="241"/>
       <c r="L19" s="37"/>
       <c r="M19" s="38"/>
     </row>
@@ -5466,14 +6597,14 @@
       <c r="C20" s="40"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
-      <c r="F20" s="214" t="s">
+      <c r="F20" s="239" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="215"/>
-      <c r="H20" s="215"/>
-      <c r="I20" s="215"/>
-      <c r="J20" s="215"/>
-      <c r="K20" s="216"/>
+      <c r="G20" s="240"/>
+      <c r="H20" s="240"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="241"/>
       <c r="L20" s="37"/>
       <c r="M20" s="38"/>
     </row>
@@ -5482,12 +6613,12 @@
       <c r="C21" s="40"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
-      <c r="F21" s="214"/>
-      <c r="G21" s="215"/>
-      <c r="H21" s="215"/>
-      <c r="I21" s="215"/>
-      <c r="J21" s="215"/>
-      <c r="K21" s="216"/>
+      <c r="F21" s="239"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="241"/>
       <c r="L21" s="37"/>
       <c r="M21" s="38"/>
     </row>
@@ -5507,12 +6638,12 @@
       <c r="C23" s="40"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
-      <c r="F23" s="217"/>
-      <c r="G23" s="218"/>
-      <c r="H23" s="218"/>
-      <c r="I23" s="218"/>
-      <c r="J23" s="218"/>
-      <c r="K23" s="219"/>
+      <c r="F23" s="242"/>
+      <c r="G23" s="243"/>
+      <c r="H23" s="243"/>
+      <c r="I23" s="243"/>
+      <c r="J23" s="243"/>
+      <c r="K23" s="244"/>
       <c r="L23" s="37"/>
       <c r="M23" s="38"/>
     </row>
@@ -5521,12 +6652,12 @@
       <c r="C24" s="40"/>
       <c r="D24" s="44"/>
       <c r="E24" s="33"/>
-      <c r="F24" s="214"/>
-      <c r="G24" s="215"/>
-      <c r="H24" s="215"/>
-      <c r="I24" s="215"/>
-      <c r="J24" s="215"/>
-      <c r="K24" s="216"/>
+      <c r="F24" s="239"/>
+      <c r="G24" s="240"/>
+      <c r="H24" s="240"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="241"/>
       <c r="L24" s="37"/>
       <c r="M24" s="38"/>
     </row>
@@ -5639,18 +6770,18 @@
       </c>
     </row>
     <row r="31" spans="2:13" ht="12.75" customHeight="1">
-      <c r="B31" s="205" t="s">
+      <c r="B31" s="230" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="206"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
-      <c r="K31" s="207"/>
+      <c r="C31" s="231"/>
+      <c r="D31" s="231"/>
+      <c r="E31" s="231"/>
+      <c r="F31" s="231"/>
+      <c r="G31" s="231"/>
+      <c r="H31" s="231"/>
+      <c r="I31" s="231"/>
+      <c r="J31" s="231"/>
+      <c r="K31" s="232"/>
       <c r="L31" s="50"/>
       <c r="M31" s="51" t="s">
         <v>28</v>
@@ -5683,18 +6814,18 @@
       </c>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="202" t="str">
+      <c r="B33" s="245" t="str">
         <f>+C4</f>
         <v>TRITURADOS BASALTICOS TEPETLAOXTOC, S.A DE C.V</v>
       </c>
-      <c r="C33" s="203"/>
-      <c r="D33" s="203"/>
-      <c r="E33" s="203"/>
-      <c r="F33" s="203"/>
-      <c r="G33" s="203"/>
-      <c r="H33" s="203"/>
-      <c r="I33" s="203"/>
-      <c r="J33" s="204"/>
+      <c r="C33" s="246"/>
+      <c r="D33" s="246"/>
+      <c r="E33" s="246"/>
+      <c r="F33" s="246"/>
+      <c r="G33" s="246"/>
+      <c r="H33" s="246"/>
+      <c r="I33" s="246"/>
+      <c r="J33" s="247"/>
       <c r="K33" s="48"/>
       <c r="L33" s="50" t="s">
         <v>28</v>
@@ -5704,21 +6835,21 @@
       </c>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="202" t="s">
+      <c r="B34" s="245" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="203"/>
-      <c r="D34" s="204"/>
-      <c r="E34" s="203" t="s">
+      <c r="C34" s="246"/>
+      <c r="D34" s="247"/>
+      <c r="E34" s="246" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="203"/>
-      <c r="G34" s="204"/>
-      <c r="H34" s="203" t="s">
+      <c r="F34" s="246"/>
+      <c r="G34" s="247"/>
+      <c r="H34" s="246" t="s">
         <v>36</v>
       </c>
-      <c r="I34" s="203"/>
-      <c r="J34" s="204"/>
+      <c r="I34" s="246"/>
+      <c r="J34" s="247"/>
       <c r="K34" s="48"/>
       <c r="L34" s="50" t="s">
         <v>28</v>
@@ -5784,19 +6915,19 @@
       <c r="M38" s="51"/>
     </row>
     <row r="39" spans="2:14">
-      <c r="B39" s="189"/>
-      <c r="C39" s="190"/>
-      <c r="D39" s="191"/>
-      <c r="E39" s="190" t="s">
+      <c r="B39" s="248"/>
+      <c r="C39" s="249"/>
+      <c r="D39" s="250"/>
+      <c r="E39" s="249" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="190"/>
-      <c r="G39" s="191"/>
-      <c r="H39" s="190" t="s">
+      <c r="F39" s="249"/>
+      <c r="G39" s="250"/>
+      <c r="H39" s="249" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="190"/>
-      <c r="J39" s="191"/>
+      <c r="I39" s="249"/>
+      <c r="J39" s="250"/>
       <c r="K39" s="79"/>
       <c r="L39" s="68" t="s">
         <v>39</v>
@@ -5807,17 +6938,17 @@
       </c>
     </row>
     <row r="40" spans="2:14">
-      <c r="B40" s="189" t="s">
+      <c r="B40" s="248" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="190"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="190"/>
-      <c r="F40" s="190"/>
-      <c r="G40" s="190"/>
-      <c r="H40" s="190"/>
-      <c r="I40" s="190"/>
-      <c r="J40" s="191"/>
+      <c r="C40" s="249"/>
+      <c r="D40" s="249"/>
+      <c r="E40" s="249"/>
+      <c r="F40" s="249"/>
+      <c r="G40" s="249"/>
+      <c r="H40" s="249"/>
+      <c r="I40" s="249"/>
+      <c r="J40" s="250"/>
       <c r="K40" s="81"/>
       <c r="L40" s="82" t="s">
         <v>41</v>
@@ -5847,14 +6978,14 @@
       <c r="B42" s="88"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
-      <c r="E42" s="192" t="s">
+      <c r="E42" s="251" t="s">
         <v>43</v>
       </c>
-      <c r="F42" s="193"/>
-      <c r="G42" s="194"/>
-      <c r="H42" s="195"/>
-      <c r="I42" s="195"/>
-      <c r="J42" s="196"/>
+      <c r="F42" s="252"/>
+      <c r="G42" s="253"/>
+      <c r="H42" s="254"/>
+      <c r="I42" s="254"/>
+      <c r="J42" s="255"/>
       <c r="K42" s="81"/>
       <c r="L42" s="82" t="s">
         <v>44</v>
@@ -5862,21 +6993,21 @@
       <c r="M42" s="80"/>
     </row>
     <row r="43" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B43" s="197" t="s">
+      <c r="B43" s="256" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="198"/>
-      <c r="D43" s="198"/>
-      <c r="E43" s="199" t="s">
+      <c r="C43" s="257"/>
+      <c r="D43" s="257"/>
+      <c r="E43" s="258" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="198"/>
-      <c r="G43" s="200"/>
-      <c r="H43" s="198" t="s">
+      <c r="F43" s="257"/>
+      <c r="G43" s="259"/>
+      <c r="H43" s="257" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="198"/>
-      <c r="J43" s="201"/>
+      <c r="I43" s="257"/>
+      <c r="J43" s="260"/>
       <c r="K43" s="89" t="s">
         <v>28</v>
       </c>
@@ -5905,12 +7036,30 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
     <mergeCell ref="F12:K13"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="L7:M7"/>
@@ -5924,30 +7073,12 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="F14:K14"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="0.82677165354330717" bottom="1" header="0.62992125984251968" footer="0"/>

</xml_diff>